<commit_message>
feat: A log message is written to the database at the time of booking
</commit_message>
<xml_diff>
--- a/logs_export.xlsx
+++ b/logs_export.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45736.58333333334</v>
+        <v>45736.77083333334</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -472,11 +472,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45737.39583333334</v>
+        <v>45736.82291666666</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>leo booked Foreign 102 3-23 8:00-3-22 10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>45739.71758101852</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2542795@dundee.ac.uk booked A311 from 2025-03-24T08:00:00 to 2025-03-24T10:00:00</t>
         </is>
       </c>
     </row>

</xml_diff>